<commit_message>
Latest Localization and Settings assets and related changes.
</commit_message>
<xml_diff>
--- a/Unity/Assets/Resources/Localization/SUGAR Unity Localization.xlsx
+++ b/Unity/Assets/Resources/Localization/SUGAR Unity Localization.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="91">
   <si>
     <t>Key</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>Login Error: {0}</t>
-  </si>
-  <si>
-    <t>{0}</t>
   </si>
   <si>
     <t>NEAR</t>
@@ -639,10 +636,10 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -936,7 +933,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>13</v>
@@ -1324,39 +1321,39 @@
         <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>13</v>
@@ -1388,10 +1385,10 @@
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>13</v>
@@ -1423,10 +1420,10 @@
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>13</v>
@@ -1458,10 +1455,10 @@
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>13</v>
@@ -1493,10 +1490,10 @@
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>13</v>
@@ -1528,10 +1525,10 @@
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>13</v>
@@ -1563,10 +1560,10 @@
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>13</v>
@@ -1598,10 +1595,10 @@
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>13</v>
@@ -1633,45 +1630,45 @@
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>13</v>
@@ -1703,10 +1700,10 @@
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>13</v>
@@ -1738,10 +1735,10 @@
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>13</v>
@@ -1773,10 +1770,10 @@
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>13</v>
@@ -1808,45 +1805,45 @@
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="C34" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>13</v>
@@ -1878,10 +1875,10 @@
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>13</v>
@@ -1913,10 +1910,10 @@
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>13</v>
@@ -1948,10 +1945,10 @@
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>13</v>
@@ -1983,10 +1980,10 @@
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>13</v>
@@ -2018,10 +2015,10 @@
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>13</v>
@@ -2056,7 +2053,7 @@
         <v>35</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>13</v>

</xml_diff>